<commit_message>
updates after Eco projects data ingest plus redevelopment stuff
</commit_message>
<xml_diff>
--- a/BackendProgress.xlsx
+++ b/BackendProgress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sea084\Dropbox\RossRCode\Git\TernLandscapes\APIs\SoilDataFederatoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35051C1D-A861-4847-8A1E-CD300AE1018B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C4EDA5-1BF4-4352-8E1C-5D974957457C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="675" windowWidth="15960" windowHeight="13545" xr2:uid="{0B932881-6185-4168-B35F-4B2F19A7FE87}"/>
+    <workbookView xWindow="4500" yWindow="1155" windowWidth="15960" windowHeight="13545" xr2:uid="{0B932881-6185-4168-B35F-4B2F19A7FE87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>Dataset</t>
   </si>
@@ -92,10 +92,22 @@
     <t>NatGeoChemicalSurvey</t>
   </si>
   <si>
-    <t>need to add al the extra data</t>
-  </si>
-  <si>
     <t>HORIZON IS THE FULL HORIZON CODE</t>
+  </si>
+  <si>
+    <t>TasGovernment</t>
+  </si>
+  <si>
+    <t>SAGovernment</t>
+  </si>
+  <si>
+    <t>EcologicalProjects</t>
+  </si>
+  <si>
+    <t>EastCentral_Australia</t>
+  </si>
+  <si>
+    <t>nssc</t>
   </si>
 </sst>
 </file>
@@ -447,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B3E278-201C-48F8-9173-34F5AEC7500C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -604,13 +616,75 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
-        <v>19</v>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>